<commit_message>
Add tab view and query param support for modules
</commit_message>
<xml_diff>
--- a/resources/graaf input.xlsx
+++ b/resources/graaf input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cf75de77b452b7ca/PRIME/prime-graaf/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="260" documentId="8_{DA69E499-F766-4593-89C5-2A511E63C18D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F4E5D18-AB17-473A-835C-AD4A86DFE1D3}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="8_{DA69E499-F766-4593-89C5-2A511E63C18D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A45B733-2B9C-47D6-BF73-E257052ABF83}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2244" windowWidth="17280" windowHeight="8964" xr2:uid="{F9F7C9D5-E42C-4BE8-9402-CE43F936AE68}"/>
+    <workbookView xWindow="1740" yWindow="1212" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{F9F7C9D5-E42C-4BE8-9402-CE43F936AE68}"/>
   </bookViews>
   <sheets>
     <sheet name="Domains" sheetId="1" r:id="rId1"/>
@@ -39,65 +39,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="65">
-  <si>
-    <t>Domain</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="64">
   <si>
     <t>Module</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>From</t>
-  </si>
-  <si>
-    <t>To</t>
-  </si>
-  <si>
     <t>Cell</t>
   </si>
   <si>
-    <t>Cell 1</t>
-  </si>
-  <si>
-    <t>Cell 2</t>
-  </si>
-  <si>
-    <t>Cell 3</t>
-  </si>
-  <si>
-    <t>Cell 4</t>
-  </si>
-  <si>
-    <t>Cell 5</t>
-  </si>
-  <si>
-    <t>Cell 6</t>
-  </si>
-  <si>
-    <t>Cell 7</t>
-  </si>
-  <si>
-    <t>Cell 8</t>
-  </si>
-  <si>
-    <t>Cell 9</t>
-  </si>
-  <si>
-    <t>Cell 10</t>
-  </si>
-  <si>
-    <t>Cell 11</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>Subspaces</t>
   </si>
   <si>
@@ -234,6 +183,54 @@
   </si>
   <si>
     <t>&lt;svg xmlns="http://www.w3.org/2000/svg" viewBox="0 0 266.46 126"&gt;&lt;defs&gt;&lt;style&gt;.cls-1{fill:#efdce3;stroke:#ae5171;stroke-miterlimit:10;stroke-width:4px;}&lt;/style&gt;&lt;/defs&gt;&lt;title&gt;symmetryMiddel 5&lt;/title&gt;&lt;g id="Laag_2" data-name="Laag 2"&gt;&lt;g id="symmetry"&gt;&lt;g id="node"&gt;&lt;polygon class="cls-1" points="234.18 2 32.28 2 2.23 63 32.28 124 234.18 124 264.23 63 234.18 2"/&gt;&lt;/g&gt;&lt;/g&gt;&lt;/g&gt;&lt;/svg&gt;</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>cell_1</t>
+  </si>
+  <si>
+    <t>cell_2</t>
+  </si>
+  <si>
+    <t>cell_3</t>
+  </si>
+  <si>
+    <t>cell_4</t>
+  </si>
+  <si>
+    <t>cell_5</t>
+  </si>
+  <si>
+    <t>cell_6</t>
+  </si>
+  <si>
+    <t>cell_7</t>
+  </si>
+  <si>
+    <t>cell_8</t>
+  </si>
+  <si>
+    <t>cell_9</t>
+  </si>
+  <si>
+    <t>cell_10</t>
+  </si>
+  <si>
+    <t>cell_11</t>
   </si>
 </sst>
 </file>
@@ -604,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D14CD2-912D-4622-A891-AC29749A8B07}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,50 +612,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -671,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD29F198-329F-4C6C-936F-5AF51F977D7B}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,291 +680,291 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1003,7 +1000,7 @@
   <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,386 +1011,386 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1411,7 +1408,7 @@
           <x14:formula1>
             <xm:f>Cells!$A$2:$A$284</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A48 B1:B1048576</xm:sqref>
+          <xm:sqref>A2:A48 B2:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1421,137 +1418,140 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29194A17-C9C1-45C2-8536-D8F51EADBDF2}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
     <col min="3" max="3" width="18" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="5.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1586,10 +1586,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add colors to links
</commit_message>
<xml_diff>
--- a/resources/graaf input.xlsx
+++ b/resources/graaf input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cf75de77b452b7ca/PRIME/prime-graaf/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="8_{DA69E499-F766-4593-89C5-2A511E63C18D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A45B733-2B9C-47D6-BF73-E257052ABF83}"/>
+  <xr:revisionPtr revIDLastSave="294" documentId="8_{DA69E499-F766-4593-89C5-2A511E63C18D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{10B6DB4F-956A-412D-B174-9808CD4CC2D1}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="1212" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{F9F7C9D5-E42C-4BE8-9402-CE43F936AE68}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F9F7C9D5-E42C-4BE8-9402-CE43F936AE68}"/>
   </bookViews>
   <sheets>
     <sheet name="Domains" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="70">
   <si>
     <t>Module</t>
   </si>
@@ -164,27 +164,12 @@
     <t>Symmetric matrices</t>
   </si>
   <si>
-    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" viewBox="0 0 266 126"&gt;&lt;defs&gt;&lt;style&gt;.cls-1{fill:#ffe2d5;stroke:#ff6c2f;stroke-miterlimit:10;stroke-width:4px;}&lt;/style&gt;&lt;/defs&gt;&lt;title&gt;Middel 1&lt;/title&gt;&lt;g id="Laag_2" data-name="Laag 2"&gt;&lt;g id="systems"&gt;&lt;g id="node_kopie_29" data-name="node kopie 29"&gt;&lt;polygon class="cls-1" points="248.1 2 17.9 2 17.1 16.34 2 16.66 2 109.34 17.1 109.66 17.9 124 248.1 124 248.9 109.66 264 109.34 264 16.66 248.9 16.34 248.1 2"/&gt;&lt;/g&gt;&lt;/g&gt;&lt;/g&gt;&lt;/svg&gt;</t>
-  </si>
-  <si>
     <t>svg</t>
   </si>
   <si>
     <t>domain</t>
   </si>
   <si>
-    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" viewBox="0 0 266 126"&gt;&lt;defs&gt;&lt;style&gt;.cls-1{fill:#fff0cf;}.cls-2{fill:none;stroke:#ffb511;stroke-miterlimit:10;stroke-width:4px;}&lt;/style&gt;&lt;/defs&gt;&lt;title&gt;eigenvaluesMiddel 1&lt;/title&gt;&lt;g id="Laag_2" data-name="Laag 2"&gt;&lt;g id="eigenvalues"&gt;&lt;g id="node_kopie_6" data-name="node kopie 6"&gt;&lt;rect class="cls-1" x="2" y="2" width="262" height="122" rx="45"/&gt;&lt;rect class="cls-2" x="2" y="2" width="262" height="122" rx="45"/&gt;&lt;/g&gt;&lt;/g&gt;&lt;/g&gt;&lt;/svg&gt;</t>
-  </si>
-  <si>
-    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" viewBox="0 0 266 126"&gt;&lt;defs&gt;&lt;style&gt;.cls-1{fill:#ffe2d5;stroke:#ff6c2f;stroke-miterlimit:10;stroke-width:4px;}&lt;/style&gt;&lt;/defs&gt;&lt;title&gt;spansMiddel 3&lt;/title&gt;&lt;g id="Laag_2" data-name="Laag 2"&gt;&lt;g id="systems"&gt;&lt;g id="node_kopie_23" data-name="node kopie 23"&gt;&lt;polygon class="cls-1" points="248.1 2 17.9 2 17.1 16.34 2 16.66 2 109.34 17.1 109.66 17.9 124 248.1 124 248.9 109.66 264 109.34 264 16.66 248.9 16.34 248.1 2"/&gt;&lt;/g&gt;&lt;/g&gt;&lt;/g&gt;&lt;/svg&gt;</t>
-  </si>
-  <si>
-    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" viewBox="0 0 266 126"&gt;&lt;defs&gt;&lt;style&gt;.cls-1{fill:#fee2e7;stroke:#f87089;stroke-miterlimit:10;stroke-width:4px;}&lt;/style&gt;&lt;/defs&gt;&lt;title&gt;transformationsMiddel 4&lt;/title&gt;&lt;g id="Laag_2" data-name="Laag 2"&gt;&lt;g id="transformations"&gt;&lt;g id="node"&gt;&lt;polygon class="cls-1" points="227.26 2 38.74 2 2 37.73 2 88.27 38.74 124 227.26 124 264 88.27 264 37.73 227.26 2"/&gt;&lt;/g&gt;&lt;/g&gt;&lt;/g&gt;&lt;/svg&gt;</t>
-  </si>
-  <si>
-    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" viewBox="0 0 266.46 126"&gt;&lt;defs&gt;&lt;style&gt;.cls-1{fill:#efdce3;stroke:#ae5171;stroke-miterlimit:10;stroke-width:4px;}&lt;/style&gt;&lt;/defs&gt;&lt;title&gt;symmetryMiddel 5&lt;/title&gt;&lt;g id="Laag_2" data-name="Laag 2"&gt;&lt;g id="symmetry"&gt;&lt;g id="node"&gt;&lt;polygon class="cls-1" points="234.18 2 32.28 2 2.23 63 32.28 124 234.18 124 264.23 63 234.18 2"/&gt;&lt;/g&gt;&lt;/g&gt;&lt;/g&gt;&lt;/svg&gt;</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -231,6 +216,39 @@
   </si>
   <si>
     <t>cell_11</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>#009DA5</t>
+  </si>
+  <si>
+    <t>#FFB511</t>
+  </si>
+  <si>
+    <t>#FF6C2F</t>
+  </si>
+  <si>
+    <t>#F87089</t>
+  </si>
+  <si>
+    <t>#AE5171</t>
+  </si>
+  <si>
+    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" preserveAspectRatio="none" viewBox="0 0 262 122"&gt;&lt;defs&gt;&lt;style&gt;.cls-1{fill:#ccebed;}.cls-2{fill:#009da5;}&lt;/style&gt;&lt;/defs&gt;&lt;title&gt;subspacesMiddel 2&lt;/title&gt;&lt;g id="Laag_2" data-name="Laag 2"&gt;&lt;g id="subspaces"&gt;&lt;g id="node_kopie_13" data-name="node kopie 13"&gt;&lt;rect class="cls-1" x="2" y="2" width="258" height="118"/&gt;&lt;path class="cls-2" d="M258,4V118H4V4H258m4-4H0V122H262V0Z"/&gt;&lt;/g&gt;&lt;/g&gt;&lt;/g&gt;&lt;/svg&gt;</t>
+  </si>
+  <si>
+    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" preserveAspectRatio="none" viewBox="0 0 266 126"&gt;&lt;defs&gt;&lt;style&gt;.cls-1{fill:#fff0cf;}.cls-2{fill:none;stroke:#ffb511;stroke-miterlimit:10;stroke-width:4px;}&lt;/style&gt;&lt;/defs&gt;&lt;title&gt;eigenvaluesMiddel 1&lt;/title&gt;&lt;g id="Laag_2" data-name="Laag 2"&gt;&lt;g id="eigenvalues"&gt;&lt;g id="node_kopie_6" data-name="node kopie 6"&gt;&lt;rect class="cls-1" x="2" y="2" width="262" height="122" rx="45"/&gt;&lt;rect class="cls-2" x="2" y="2" width="262" height="122" rx="45"/&gt;&lt;/g&gt;&lt;/g&gt;&lt;/g&gt;&lt;/svg&gt;</t>
+  </si>
+  <si>
+    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" preserveAspectRatio="none" viewBox="0 0 266 126"&gt;&lt;defs&gt;&lt;style&gt;.cls-1{fill:#ffe2d5;stroke:#ff6c2f;stroke-miterlimit:10;stroke-width:4px;}&lt;/style&gt;&lt;/defs&gt;&lt;title&gt;spansMiddel 3&lt;/title&gt;&lt;g id="Laag_2" data-name="Laag 2"&gt;&lt;g id="systems"&gt;&lt;g id="node_kopie_23" data-name="node kopie 23"&gt;&lt;polygon class="cls-1" points="248.1 2 17.9 2 17.1 16.34 2 16.66 2 109.34 17.1 109.66 17.9 124 248.1 124 248.9 109.66 264 109.34 264 16.66 248.9 16.34 248.1 2"/&gt;&lt;/g&gt;&lt;/g&gt;&lt;/g&gt;&lt;/svg&gt;</t>
+  </si>
+  <si>
+    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" preserveAspectRatio="none" viewBox="0 0 266 126"&gt;&lt;defs&gt;&lt;style&gt;.cls-1{fill:#fee2e7;stroke:#f87089;stroke-miterlimit:10;stroke-width:4px;}&lt;/style&gt;&lt;/defs&gt;&lt;title&gt;transformationsMiddel 4&lt;/title&gt;&lt;g id="Laag_2" data-name="Laag 2"&gt;&lt;g id="transformations"&gt;&lt;g id="node"&gt;&lt;polygon class="cls-1" points="227.26 2 38.74 2 2 37.73 2 88.27 38.74 124 227.26 124 264 88.27 264 37.73 227.26 2"/&gt;&lt;/g&gt;&lt;/g&gt;&lt;/g&gt;&lt;/svg&gt;</t>
+  </si>
+  <si>
+    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" preserveAspectRatio="none" viewBox="0 0 266.46 126"&gt;&lt;defs&gt;&lt;style&gt;.cls-1{fill:#efdce3;stroke:#ae5171;stroke-miterlimit:10;stroke-width:4px;}&lt;/style&gt;&lt;/defs&gt;&lt;title&gt;symmetryMiddel 5&lt;/title&gt;&lt;g id="Laag_2" data-name="Laag 2"&gt;&lt;g id="symmetry"&gt;&lt;g id="node"&gt;&lt;polygon class="cls-1" points="234.18 2 32.28 2 2.23 63 32.28 124 234.18 124 264.23 63 234.18 2"/&gt;&lt;/g&gt;&lt;/g&gt;&lt;/g&gt;&lt;/svg&gt;</t>
   </si>
 </sst>
 </file>
@@ -599,63 +617,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D14CD2-912D-4622-A891-AC29749A8B07}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -680,10 +717,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -1011,10 +1048,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1420,7 +1457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29194A17-C9C1-45C2-8536-D8F51EADBDF2}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1436,43 +1473,43 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="N1" s="1"/>
     </row>

</xml_diff>

<commit_message>
Change module to lecture
</commit_message>
<xml_diff>
--- a/resources/graaf input.xlsx
+++ b/resources/graaf input.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cf75de77b452b7ca/PRIME/prime-graaf/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="294" documentId="8_{DA69E499-F766-4593-89C5-2A511E63C18D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{10B6DB4F-956A-412D-B174-9808CD4CC2D1}"/>
+  <xr:revisionPtr revIDLastSave="296" documentId="8_{DA69E499-F766-4593-89C5-2A511E63C18D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BC46DC25-0F14-4458-B28A-F2E98C7F871A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F9F7C9D5-E42C-4BE8-9402-CE43F936AE68}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{F9F7C9D5-E42C-4BE8-9402-CE43F936AE68}"/>
   </bookViews>
   <sheets>
     <sheet name="Domains" sheetId="1" r:id="rId1"/>
     <sheet name="Cells" sheetId="3" r:id="rId2"/>
     <sheet name="Edges" sheetId="4" r:id="rId3"/>
-    <sheet name="Modules" sheetId="2" r:id="rId4"/>
+    <sheet name="Lectures" sheetId="2" r:id="rId4"/>
     <sheet name="Cell-Module" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
@@ -619,7 +619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D14CD2-912D-4622-A891-AC29749A8B07}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1022,7 +1022,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{96EE9631-BF88-4B4B-B761-D4C95E479831}">
           <x14:formula1>
-            <xm:f>Modules!$A$2:$A$11</xm:f>
+            <xm:f>Lectures!$A$2:$A$11</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C39</xm:sqref>
         </x14:dataValidation>
@@ -1457,7 +1457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29194A17-C9C1-45C2-8536-D8F51EADBDF2}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>